<commit_message>
Airport commit. Trying to get lua filters to work. It still does not bold author name.
</commit_message>
<xml_diff>
--- a/docs/education_bar.xlsx
+++ b/docs/education_bar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\CVR_BAR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4675DE7B-3BF0-4452-A4A2-8A67B0DD6099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B28182-4F86-453E-8F20-03F3EF01EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,18 +83,39 @@
     <t>Bachelor of Arts in Political Science,</t>
   </si>
   <si>
-    <t>Area of concentration: Political Theory, *Magna Cum Laude*</t>
-  </si>
-  <si>
     <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P.Camilo Zalamea, Ph.D.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Area of concentration: Political Theory, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Magna Cum Laude</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -441,16 +462,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" customWidth="1"/>
+    <col min="1" max="1" width="63.453125" customWidth="1"/>
     <col min="2" max="2" width="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -481,12 +502,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -500,7 +521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -514,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes modeled after L. Abad's CV
</commit_message>
<xml_diff>
--- a/docs/education_bar.xlsx
+++ b/docs/education_bar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\CVR_BAR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B28182-4F86-453E-8F20-03F3EF01EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C52CCB-0FC8-4C98-A24A-BBFB34418ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11265" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Bachelor of Arts in Political Science,</t>
   </si>
   <si>
-    <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P.Camilo Zalamea, Ph.D.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Area of concentration: Political Theory, </t>
     </r>
@@ -100,6 +97,9 @@
       </rPr>
       <t>Magna Cum Laude</t>
     </r>
+  </si>
+  <si>
+    <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P. Camilo Zalamea, Ph.D.</t>
   </si>
 </sst>
 </file>
@@ -462,16 +462,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.453125" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
     <col min="2" max="2" width="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -502,12 +502,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -521,7 +521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -535,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes modeled after L. Abad CV
</commit_message>
<xml_diff>
--- a/docs/education_bar.xlsx
+++ b/docs/education_bar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\CVR_BAR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B28182-4F86-453E-8F20-03F3EF01EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C52CCB-0FC8-4C98-A24A-BBFB34418ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11265" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Bachelor of Arts in Political Science,</t>
   </si>
   <si>
-    <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P.Camilo Zalamea, Ph.D.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Area of concentration: Political Theory, </t>
     </r>
@@ -100,6 +97,9 @@
       </rPr>
       <t>Magna Cum Laude</t>
     </r>
+  </si>
+  <si>
+    <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P. Camilo Zalamea, Ph.D.</t>
   </si>
 </sst>
 </file>
@@ -462,16 +462,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.453125" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
     <col min="2" max="2" width="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -502,12 +502,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -521,7 +521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -535,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing formatting through .cls file. Attempt at Lua filter for scientific names.
</commit_message>
<xml_diff>
--- a/docs/education_bar.xlsx
+++ b/docs/education_bar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\CVR_BAR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C52CCB-0FC8-4C98-A24A-BBFB34418ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5957C401-E45B-400E-A7DA-D3F249EFE105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11265" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{A97DD69B-DFA4-4E39-9D50-C97A7E8500B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">2018 - Present    </t>
   </si>
   <si>
-    <t>Master of Science, Natural Resources Management: Conservation Ecology,</t>
-  </si>
-  <si>
     <t>Ph. D. candidate in Ecology and Evolutionary Biology</t>
   </si>
   <si>
@@ -68,16 +65,7 @@
     <t>Ann Arbor, MI</t>
   </si>
   <si>
-    <t>University of Puerto Rico</t>
-  </si>
-  <si>
     <t>San Juan, Puerto Rico</t>
-  </si>
-  <si>
-    <t>Tulane University, Department of Ecology and Biology</t>
-  </si>
-  <si>
-    <t>University of Michigan, School for the Environment and Sustainability</t>
   </si>
   <si>
     <t>Bachelor of Arts in Political Science,</t>
@@ -99,7 +87,19 @@
     </r>
   </si>
   <si>
-    <t>Committee members: Sunshine Van Bael, Ph.D. (adviser; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P. Camilo Zalamea, Ph.D.</t>
+    <t>Tulane University (TU), Department of Ecology and Biology</t>
+  </si>
+  <si>
+    <t>University of Michigan (UM), School for the Environment and Sustainability</t>
+  </si>
+  <si>
+    <t>University of Puerto Rico (UPR)</t>
+  </si>
+  <si>
+    <t>Committee members: Sunshine Van Bael, Ph.D. (advisor; dissertation chair), Kathleen Ferris, Ph.D.  (co-advisor), Keith Clay, Ph.D., &amp; P. Camilo Zalamea, Ph.D.</t>
+  </si>
+  <si>
+    <t>Master of Science, Natural Resources Management: Conservation Ecology</t>
   </si>
 </sst>
 </file>
@@ -462,16 +462,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" customWidth="1"/>
-    <col min="2" max="2" width="86" customWidth="1"/>
+    <col min="1" max="1" width="63.3984375" customWidth="1"/>
+    <col min="2" max="2" width="41.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,9 +488,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -499,17 +499,17 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
       </c>
       <c r="B4">
         <v>2018</v>
@@ -518,24 +518,24 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2014</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>